<commit_message>
New Changes has been added which includes Future prediction
</commit_message>
<xml_diff>
--- a/DPMMVCCore/DPM_Testing/wwwroot/DPM/src/assets/Excel_Format.xlsx
+++ b/DPMMVCCore/DPM_Testing/wwwroot/DPM/src/assets/Excel_Format.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AminSohail\Desktop\DPM\DPM\src\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\DPM References\DPM Version 2\DPMCore\DPMMVCCore\DPM_Testing\wwwroot\DPM\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{567A056B-AC05-45A0-839A-088B73A272F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="20730" windowHeight="11310" xr2:uid="{BD3579F7-E392-46B6-B615-A02DD36C2380}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="20730" windowHeight="11310"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>PS1</t>
   </si>
@@ -49,12 +48,15 @@
   </si>
   <si>
     <t>TD2</t>
+  </si>
+  <si>
+    <t>InsertedDate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -413,16 +415,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1198272D-C668-4CCA-A7E1-11BDDF01718C}">
-  <dimension ref="A1:H1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -446,6 +448,9 @@
       </c>
       <c r="H1" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>